<commit_message>
Se arreglo generacion de electricidad
</commit_message>
<xml_diff>
--- a/DataBases/BI - Capacidad de Autogeneracion.xlsx
+++ b/DataBases/BI - Capacidad de Autogeneracion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JULIAN\Music\TIMES-UIS-v1-Nov\DataBases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E43877-CD9D-4F2C-9005-EABAC4F3345C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECCC209-8CCA-43B4-80A0-67A5A2AB4C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Autogeneracion Fuels" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>JULIAN:</t>
         </r>
@@ -63,7 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Edgar</t>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>JULIAN:</t>
         </r>
@@ -87,7 +87,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Ecopetrol, Hocol, y Meta Petroleum
@@ -113,7 +113,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>JULIAN:</t>
         </r>
@@ -122,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Edgar</t>
@@ -137,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>JULIAN:</t>
         </r>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Ecopetrol, Hocol, y Meta Petroleum
@@ -159,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="172">
   <si>
     <t>Sector Petróleo</t>
   </si>
@@ -672,6 +672,9 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>Consumo</t>
   </si>
 </sst>
 </file>
@@ -710,14 +713,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -930,7 +933,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -962,22 +965,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -989,19 +979,16 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1035,7 +1022,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1053,23 +1040,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1078,15 +1061,15 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1098,7 +1081,29 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1107,6 +1112,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1117,21 +1128,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1778,12 +1774,12 @@
       <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="G20" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
+      <c r="H20" s="79"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
       <c r="K20" t="s">
         <v>20</v>
       </c>
@@ -2026,17 +2022,17 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="80"/>
+      <c r="I31" s="80"/>
+      <c r="J31" s="80"/>
     </row>
     <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
@@ -2077,33 +2073,33 @@
       <c r="E37" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H37" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="19"/>
-      <c r="J37" s="19" t="s">
+      <c r="I37" s="79"/>
+      <c r="J37" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="K37" s="19"/>
-      <c r="L37" s="19" t="s">
+      <c r="K37" s="79"/>
+      <c r="L37" s="79" t="s">
         <v>110</v>
       </c>
-      <c r="M37" s="19"/>
-      <c r="N37" s="19" t="s">
+      <c r="M37" s="79"/>
+      <c r="N37" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="O37" s="19"/>
-      <c r="P37" s="19"/>
-      <c r="Q37" s="19" t="s">
+      <c r="O37" s="79"/>
+      <c r="P37" s="79"/>
+      <c r="Q37" s="79" t="s">
         <v>111</v>
       </c>
-      <c r="R37" s="19"/>
-      <c r="S37" s="19" t="s">
+      <c r="R37" s="79"/>
+      <c r="S37" s="79" t="s">
         <v>107</v>
       </c>
-      <c r="T37" s="19"/>
-      <c r="U37" s="19"/>
-      <c r="V37" s="19"/>
+      <c r="T37" s="79"/>
+      <c r="U37" s="79"/>
+      <c r="V37" s="79"/>
     </row>
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -2693,11 +2689,11 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I55" s="19" t="s">
+      <c r="I55" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
+      <c r="J55" s="79"/>
+      <c r="K55" s="79"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
@@ -2798,8 +2794,8 @@
   </sheetPr>
   <dimension ref="A1:AR41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="N1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView showGridLines="0" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2824,31 +2820,31 @@
       <c r="A1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="U1" s="74"/>
-      <c r="V1" s="80" t="s">
+      <c r="U1" s="66"/>
+      <c r="V1" s="82" t="s">
         <v>168</v>
       </c>
-      <c r="W1" s="81"/>
-      <c r="X1" s="81"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="79"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="66"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C2" s="9"/>
-      <c r="U2" s="74"/>
-      <c r="V2" s="75" t="s">
+      <c r="U2" s="66"/>
+      <c r="V2" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="W2" s="76" t="s">
+      <c r="W2" s="68" t="s">
         <v>144</v>
       </c>
-      <c r="X2" s="76" t="s">
+      <c r="X2" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="Y2" s="76" t="s">
+      <c r="Y2" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="Z2" s="74"/>
+      <c r="Z2" s="66"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C3" s="9" t="s">
@@ -2857,26 +2853,26 @@
       <c r="D3" s="2">
         <v>0.35</v>
       </c>
-      <c r="U3" s="74" t="s">
+      <c r="U3" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="77">
+      <c r="V3" s="69">
         <f>+(V17*0.35*1000/0.0036)/(365*24)</f>
         <v>19.999999999999996</v>
       </c>
-      <c r="W3" s="77">
+      <c r="W3" s="69">
         <f t="shared" ref="W3:Y3" si="0">+(W17*0.35*1000/0.0036)/(365*24)</f>
         <v>150.07647247502405</v>
       </c>
-      <c r="X3" s="77">
+      <c r="X3" s="69">
         <f t="shared" si="0"/>
         <v>48.264281002198075</v>
       </c>
-      <c r="Y3" s="77">
+      <c r="Y3" s="69">
         <f t="shared" si="0"/>
         <v>22.809206522777917</v>
       </c>
-      <c r="Z3" s="74"/>
+      <c r="Z3" s="66"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C4" s="9" t="s">
@@ -2885,49 +2881,49 @@
       <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="V4" s="77">
+      <c r="V4" s="69">
         <f t="shared" ref="V4:Y4" si="1">+(V18*0.35*1000/0.0036)/(365*24)</f>
         <v>0</v>
       </c>
-      <c r="W4" s="77">
+      <c r="W4" s="69">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="X4" s="77">
+      <c r="X4" s="69">
         <f t="shared" si="1"/>
         <v>21.228029807445445</v>
       </c>
-      <c r="Y4" s="77">
+      <c r="Y4" s="69">
         <f t="shared" si="1"/>
         <v>10.032150192554559</v>
       </c>
-      <c r="Z4" s="74"/>
+      <c r="Z4" s="66"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C5" s="9"/>
-      <c r="U5" s="74" t="s">
+      <c r="U5" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="V5" s="77">
+      <c r="V5" s="69">
         <f t="shared" ref="V5:Y5" si="2">+(V19*0.35*1000/0.0036)/(365*24)</f>
         <v>0</v>
       </c>
-      <c r="W5" s="77">
+      <c r="W5" s="69">
         <f t="shared" si="2"/>
         <v>19.445743599518565</v>
       </c>
-      <c r="X5" s="77">
+      <c r="X5" s="69">
         <f t="shared" si="2"/>
         <v>41.381229673754405</v>
       </c>
-      <c r="Y5" s="77">
+      <c r="Y5" s="69">
         <f t="shared" si="2"/>
         <v>19.556346726727035</v>
       </c>
-      <c r="Z5" s="74"/>
+      <c r="Z5" s="66"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="C6" s="9" t="s">
@@ -2937,48 +2933,48 @@
         <f>30.9%+22.8%+2.9%</f>
         <v>0.56600000000000006</v>
       </c>
-      <c r="U6" s="74" t="s">
+      <c r="U6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="V6" s="77">
+      <c r="V6" s="69">
         <f t="shared" ref="V6:Y6" si="3">+(V20*0.35*1000/0.0036)/(365*24)</f>
         <v>0</v>
       </c>
-      <c r="W6" s="77">
+      <c r="W6" s="69">
         <f t="shared" si="3"/>
         <v>2.2835888766070749</v>
       </c>
-      <c r="X6" s="77">
+      <c r="X6" s="69">
         <f t="shared" si="3"/>
         <v>19.677300005487623</v>
       </c>
-      <c r="Y6" s="77">
+      <c r="Y6" s="69">
         <f t="shared" si="3"/>
         <v>9.2992911179053053</v>
       </c>
-      <c r="Z6" s="74"/>
+      <c r="Z6" s="66"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="U7" s="78" t="s">
+      <c r="U7" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="V7" s="77">
+      <c r="V7" s="69">
         <f t="shared" ref="V7:Y7" si="4">+(V21*0.35*1000/0.0036)/(365*24)</f>
         <v>0</v>
       </c>
-      <c r="W7" s="77">
+      <c r="W7" s="69">
         <f t="shared" si="4"/>
         <v>0.25423007512003598</v>
       </c>
-      <c r="X7" s="77">
+      <c r="X7" s="69">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="77">
+      <c r="Y7" s="69">
         <f t="shared" si="4"/>
         <v>8.8787417554540831</v>
       </c>
-      <c r="Z7" s="74"/>
+      <c r="Z7" s="66"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="V8" s="7"/>
@@ -2988,10 +2984,10 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="10" t="s">
         <v>121</v>
       </c>
@@ -3000,6 +2996,7 @@
         <v>122</v>
       </c>
       <c r="H9" s="10"/>
+      <c r="V9" s="7"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
@@ -3037,10 +3034,10 @@
       <c r="I11" s="4"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="79"/>
       <c r="E12" t="s">
         <v>121</v>
       </c>
@@ -3083,13 +3080,13 @@
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="V14" s="52" t="s">
+      <c r="V14" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="W14" s="52"/>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="52"/>
+      <c r="W14" s="81"/>
+      <c r="X14" s="81"/>
+      <c r="Y14" s="81"/>
+      <c r="Z14" s="81"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="L15" s="3"/>
@@ -3124,68 +3121,68 @@
       <c r="C16" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="E16" s="22"/>
-      <c r="H16" s="22" t="s">
+      <c r="E16" s="86"/>
+      <c r="H16" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="I16" s="22"/>
+      <c r="I16" s="86"/>
       <c r="L16" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22" t="s">
+      <c r="N16" s="86"/>
+      <c r="O16" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="P16" s="22"/>
+      <c r="P16" s="86"/>
       <c r="R16" s="12" t="s">
         <v>155</v>
       </c>
       <c r="S16" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="V16" s="28" t="s">
+      <c r="V16" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="W16" s="25" t="s">
+      <c r="W16" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="X16" s="25" t="s">
+      <c r="X16" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="Y16" s="25" t="s">
+      <c r="Y16" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="Z16" s="49" t="s">
+      <c r="Z16" s="43" t="s">
         <v>158</v>
       </c>
-      <c r="AD16" s="28" t="s">
+      <c r="AD16" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="AE16" s="25" t="s">
+      <c r="AE16" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="AF16" s="25" t="s">
+      <c r="AF16" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="AG16" s="25" t="s">
+      <c r="AG16" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="AI16" s="28" t="s">
+      <c r="AI16" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="AJ16" s="25" t="s">
+      <c r="AJ16" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="AK16" s="25" t="s">
+      <c r="AK16" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="AL16" s="25" t="s">
+      <c r="AL16" s="20" t="s">
         <v>113</v>
       </c>
       <c r="AM16" s="12" t="s">
@@ -3247,58 +3244,58 @@
         <f>+R17-M17</f>
         <v>7.6443192183346502</v>
       </c>
-      <c r="V17" s="29">
+      <c r="V17" s="24">
         <f>+(20*24*0.365)*0.0036/D3</f>
         <v>1.8020571428571428</v>
       </c>
-      <c r="W17" s="34">
+      <c r="W17" s="28">
         <f>+((H34-AE23)*24*0.365)*0.0036/D3</f>
         <v>13.522318959921025</v>
       </c>
-      <c r="X17" s="34">
+      <c r="X17" s="28">
         <f>+Z17-Y17</f>
         <v>4.3487496162437669</v>
       </c>
-      <c r="Y17" s="34">
+      <c r="Y17" s="28">
         <f>+Z17/(2.116+1)</f>
         <v>2.0551746768637837</v>
       </c>
-      <c r="Z17" s="47">
+      <c r="Z17" s="41">
         <v>6.4039242931075506</v>
       </c>
       <c r="AA17">
         <f>+Z17/0.0036</f>
         <v>1778.867859196542</v>
       </c>
-      <c r="AD17" s="40">
+      <c r="AD17" s="34">
         <f>+(V17*0.35/0.0036)*1000/(24*365)</f>
         <v>20</v>
       </c>
-      <c r="AE17" s="41">
+      <c r="AE17" s="35">
         <f>+H34-AE23</f>
         <v>150.07647247502405</v>
       </c>
-      <c r="AF17" s="30">
-        <f>+(X17*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AF17" s="13">
+        <f t="shared" ref="AF17:AG21" si="6">+(X17*0.35/0.0036)*1000/(24*365)</f>
         <v>48.264281002198068</v>
       </c>
-      <c r="AG17" s="30">
-        <f>+(Y17*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AG17" s="13">
+        <f t="shared" si="6"/>
         <v>22.809206522777917</v>
       </c>
-      <c r="AI17" s="45">
-        <f>+V17*0.35</f>
+      <c r="AI17" s="39">
+        <f t="shared" ref="AI17:AK21" si="7">+V17*0.35</f>
         <v>0.63071999999999995</v>
       </c>
-      <c r="AJ17" s="41">
-        <f>+W17*0.35</f>
+      <c r="AJ17" s="35">
+        <f t="shared" si="7"/>
         <v>4.7328116359723582</v>
       </c>
-      <c r="AK17" s="30">
-        <f>+X17*0.35</f>
+      <c r="AK17" s="13">
+        <f t="shared" si="7"/>
         <v>1.5220623656853183</v>
       </c>
-      <c r="AL17" s="30">
+      <c r="AL17" s="13">
         <v>0</v>
       </c>
       <c r="AM17" s="7">
@@ -3338,7 +3335,7 @@
         <v>6</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" ref="H18:H21" si="6">+SUMIF($A$17:$A$30,G18,$D$17:$D$30)</f>
+        <f t="shared" ref="H18:H21" si="8">+SUMIF($A$17:$A$30,G18,$D$17:$D$30)</f>
         <v>31.260180000000009</v>
       </c>
       <c r="I18" t="s">
@@ -3355,7 +3352,7 @@
         <v>19</v>
       </c>
       <c r="O18" s="6">
-        <f t="shared" ref="O18:O22" si="7">+M18/$D$3</f>
+        <f t="shared" ref="O18:O22" si="9">+M18/$D$3</f>
         <v>2.8166315328000007</v>
       </c>
       <c r="P18" t="s">
@@ -3369,56 +3366,56 @@
         <f>+R18-M18</f>
         <v>-0.87656533364335421</v>
       </c>
-      <c r="V18" s="29">
+      <c r="V18" s="24">
         <v>0</v>
       </c>
-      <c r="W18" s="34">
+      <c r="W18" s="28">
         <v>0</v>
       </c>
-      <c r="X18" s="34">
-        <f t="shared" ref="X18:X20" si="8">+Z18-Y18</f>
+      <c r="X18" s="28">
+        <f t="shared" ref="X18:X20" si="10">+Z18-Y18</f>
         <v>1.9127061371645704</v>
       </c>
-      <c r="Y18" s="34">
-        <f t="shared" ref="Y18:Y20" si="9">+Z18/(2.116+1)</f>
+      <c r="Y18" s="28">
+        <f t="shared" ref="Y18:Y20" si="11">+Z18/(2.116+1)</f>
         <v>0.90392539563543017</v>
       </c>
-      <c r="Z18" s="47">
+      <c r="Z18" s="41">
         <v>2.8166315328000007</v>
       </c>
       <c r="AA18">
-        <f t="shared" ref="AA18:AA21" si="10">+Z18/0.0036</f>
+        <f t="shared" ref="AA18:AA21" si="12">+Z18/0.0036</f>
         <v>782.39764800000023</v>
       </c>
-      <c r="AD18" s="29">
+      <c r="AD18" s="24">
         <f>+(V18*0.35/0.0036)*1000/(24*365)</f>
         <v>0</v>
       </c>
-      <c r="AE18" s="42">
+      <c r="AE18" s="36">
         <f>+(W18*0.35/0.0036)*1000/(24*365)</f>
         <v>0</v>
       </c>
-      <c r="AF18" s="30">
-        <f>+(X18*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AF18" s="13">
+        <f t="shared" si="6"/>
         <v>21.228029807445449</v>
       </c>
-      <c r="AG18" s="30">
-        <f>+(Y18*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AG18" s="13">
+        <f t="shared" si="6"/>
         <v>10.032150192554559</v>
       </c>
-      <c r="AI18" s="29">
-        <f>+V18*0.35</f>
+      <c r="AI18" s="24">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AJ18" s="42">
-        <f>+W18*0.35</f>
+      <c r="AJ18" s="36">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AK18" s="30">
-        <f>+X18*0.35</f>
+      <c r="AK18" s="13">
+        <f t="shared" si="7"/>
         <v>0.66944714800759964</v>
       </c>
-      <c r="AL18" s="30">
+      <c r="AL18" s="13">
         <f>+Y18*0.35</f>
         <v>0.31637388847240056</v>
       </c>
@@ -3449,7 +3446,7 @@
         <v>0.11</v>
       </c>
       <c r="D19" s="4">
-        <f t="shared" ref="D19:D30" si="11">+C19*$C$13</f>
+        <f t="shared" ref="D19:D30" si="13">+C19*$C$13</f>
         <v>49.123140000000006</v>
       </c>
       <c r="E19" t="s">
@@ -3459,7 +3456,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>80.383320000000012</v>
       </c>
       <c r="I19" t="s">
@@ -3476,7 +3473,7 @@
         <v>19</v>
       </c>
       <c r="O19" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>7.2427667986285718</v>
       </c>
       <c r="P19" t="s">
@@ -3490,56 +3487,56 @@
         <f>+R19-M19</f>
         <v>-4.2026667786310146E-2</v>
       </c>
-      <c r="V19" s="29">
+      <c r="V19" s="24">
         <v>0</v>
       </c>
-      <c r="W19" s="34">
+      <c r="W19" s="28">
         <v>1.7521170575840499</v>
       </c>
-      <c r="X19" s="34">
-        <f t="shared" si="8"/>
+      <c r="X19" s="28">
+        <f t="shared" si="10"/>
         <v>3.7285670256900545</v>
       </c>
-      <c r="Y19" s="34">
-        <f t="shared" si="9"/>
+      <c r="Y19" s="28">
+        <f t="shared" si="11"/>
         <v>1.7620827153544678</v>
       </c>
-      <c r="Z19" s="47">
+      <c r="Z19" s="41">
         <v>5.4906497410445221</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1525.1804836234785</v>
       </c>
-      <c r="AD19" s="29">
+      <c r="AD19" s="24">
         <f>+(V19*0.35/0.0036)*1000/(24*365)</f>
         <v>0</v>
       </c>
-      <c r="AE19" s="42">
+      <c r="AE19" s="36">
         <f>+(W19*0.35/0.0036)*1000/(24*365)</f>
         <v>19.445743599518565</v>
       </c>
-      <c r="AF19" s="30">
-        <f>+(X19*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AF19" s="13">
+        <f t="shared" si="6"/>
         <v>41.381229673754405</v>
       </c>
-      <c r="AG19" s="30">
-        <f>+(Y19*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AG19" s="13">
+        <f t="shared" si="6"/>
         <v>19.556346726727032</v>
       </c>
-      <c r="AI19" s="29">
-        <f>+V19*0.35</f>
+      <c r="AI19" s="24">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AJ19" s="42">
-        <f>+W19*0.35</f>
+      <c r="AJ19" s="36">
+        <f t="shared" si="7"/>
         <v>0.61324097015441748</v>
       </c>
-      <c r="AK19" s="30">
-        <f>+X19*0.35</f>
+      <c r="AK19" s="13">
+        <f t="shared" si="7"/>
         <v>1.3049984589915189</v>
       </c>
-      <c r="AL19" s="30">
+      <c r="AL19" s="13">
         <f>+Y19*0.35</f>
         <v>0.61672895037406372</v>
       </c>
@@ -3552,7 +3549,7 @@
         <v>2.4929417117336898</v>
       </c>
       <c r="AQ19">
-        <f t="shared" ref="AQ19:AQ21" si="12">+(AO19-AM19)/0.0036</f>
+        <f t="shared" ref="AQ19:AQ21" si="14">+(AO19-AM19)/0.0036</f>
         <v>-11.674074385086152</v>
       </c>
       <c r="AR19" t="s">
@@ -3570,7 +3567,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D20" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31.260180000000009</v>
       </c>
       <c r="E20" t="s">
@@ -3580,7 +3577,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>31.260180000000009</v>
       </c>
       <c r="I20" t="s">
@@ -3590,14 +3587,14 @@
         <v>5</v>
       </c>
       <c r="M20" s="7">
-        <f t="shared" ref="M20:M21" si="13">+H20*$D$4*24*365*0.0036/1000</f>
+        <f t="shared" ref="M20:M21" si="15">+H20*$D$4*24*365*0.0036/1000</f>
         <v>0.98582103648000019</v>
       </c>
       <c r="N20" t="s">
         <v>19</v>
       </c>
       <c r="O20" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8166315328000007</v>
       </c>
       <c r="P20" t="s">
@@ -3611,56 +3608,56 @@
         <f>+R20-M20</f>
         <v>-0.53428021051158625</v>
       </c>
-      <c r="V20" s="29">
+      <c r="V20" s="24">
         <v>0</v>
       </c>
-      <c r="W20" s="34">
+      <c r="W20" s="28">
         <v>0.20575788232194489</v>
       </c>
-      <c r="X20" s="34">
-        <f t="shared" si="8"/>
+      <c r="X20" s="28">
+        <f t="shared" si="10"/>
         <v>1.7729809513515935</v>
       </c>
-      <c r="Y20" s="34">
-        <f t="shared" si="9"/>
+      <c r="Y20" s="28">
+        <f t="shared" si="11"/>
         <v>0.83789269912646203</v>
       </c>
-      <c r="Z20" s="47">
+      <c r="Z20" s="41">
         <v>2.6108736504780556</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>725.24268068834886</v>
       </c>
-      <c r="AD20" s="29">
+      <c r="AD20" s="24">
         <f>+(V20*0.35/0.0036)*1000/(24*365)</f>
         <v>0</v>
       </c>
-      <c r="AE20" s="42">
+      <c r="AE20" s="36">
         <f>+(W20*0.35/0.0036)*1000/(24*365)</f>
         <v>2.2835888766070749</v>
       </c>
-      <c r="AF20" s="33">
-        <f>+(X20*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AF20" s="27">
+        <f t="shared" si="6"/>
         <v>19.677300005487627</v>
       </c>
-      <c r="AG20" s="30">
-        <f>+(Y20*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AG20" s="13">
+        <f t="shared" si="6"/>
         <v>9.2992911179053053</v>
       </c>
-      <c r="AI20" s="29">
-        <f>+V20*0.35</f>
+      <c r="AI20" s="24">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AJ20" s="42">
-        <f>+W20*0.35</f>
+      <c r="AJ20" s="36">
+        <f t="shared" si="7"/>
         <v>7.2015258812680713E-2</v>
       </c>
-      <c r="AK20" s="46">
-        <f>+X20*0.35</f>
+      <c r="AK20" s="40">
+        <f t="shared" si="7"/>
         <v>0.62054333297305764</v>
       </c>
-      <c r="AL20" s="30">
+      <c r="AL20" s="13">
         <f>+Y20*0.35</f>
         <v>0.29326244469426171</v>
       </c>
@@ -3673,7 +3670,7 @@
         <v>0.45154082596841399</v>
       </c>
       <c r="AQ20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-148.41116958655167</v>
       </c>
       <c r="AR20" t="s">
@@ -3691,7 +3688,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>31.260180000000009</v>
       </c>
       <c r="E21" t="s">
@@ -3701,7 +3698,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>8.9314800000000023</v>
       </c>
       <c r="I21" s="14" t="s">
@@ -3711,21 +3708,20 @@
         <v>4</v>
       </c>
       <c r="M21" s="15">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.28166315328000008</v>
       </c>
       <c r="N21" s="14" t="s">
         <v>19</v>
       </c>
       <c r="O21" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.80475186651428599</v>
       </c>
       <c r="P21" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24">
+      <c r="R21">
         <f>+Hoja1!G78</f>
         <v>0.13373317447933</v>
       </c>
@@ -3733,55 +3729,54 @@
         <f>+R21-M21</f>
         <v>-0.14792997880067008</v>
       </c>
-      <c r="T21" s="24"/>
-      <c r="V21" s="31">
+      <c r="V21" s="25">
         <v>0</v>
       </c>
-      <c r="W21" s="35">
+      <c r="W21" s="29">
         <v>2.2906856139958444E-2</v>
       </c>
-      <c r="X21" s="35">
+      <c r="X21" s="29">
         <v>0</v>
       </c>
-      <c r="Y21" s="35">
+      <c r="Y21" s="29">
         <v>0.8</v>
       </c>
-      <c r="Z21" s="48">
+      <c r="Z21" s="42">
         <v>0.78184501037432752</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>217.17916954842431</v>
       </c>
-      <c r="AD21" s="31">
+      <c r="AD21" s="25">
         <f>+(V21*0.35/0.0036)*1000/(24*365)</f>
         <v>0</v>
       </c>
-      <c r="AE21" s="43">
+      <c r="AE21" s="37">
         <f>+(W21*0.35/0.0036)*1000/(24*365)</f>
         <v>0.25423007512003598</v>
       </c>
-      <c r="AF21" s="32">
-        <f>+(X21*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AF21" s="26">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="AG21" s="32">
-        <f>+(Y21*0.35/0.0036)*1000/(24*365)</f>
+      <c r="AG21" s="26">
+        <f t="shared" si="6"/>
         <v>8.8787417554540831</v>
       </c>
-      <c r="AI21" s="31">
-        <f>+V21*0.35</f>
+      <c r="AI21" s="25">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AJ21" s="43">
-        <f>+W21*0.35</f>
+      <c r="AJ21" s="37">
+        <f t="shared" si="7"/>
         <v>8.0173996489854554E-3</v>
       </c>
-      <c r="AK21" s="44">
-        <f>+X21*0.35</f>
+      <c r="AK21" s="38">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AL21" s="32">
+      <c r="AL21" s="26">
         <f>+Y21*0.35</f>
         <v>0.27999999999999997</v>
       </c>
@@ -3794,7 +3789,7 @@
         <v>0.13373317447933</v>
       </c>
       <c r="AQ21">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-42.856729213793173</v>
       </c>
       <c r="AR21" t="s">
@@ -3812,7 +3807,7 @@
         <v>0.05</v>
       </c>
       <c r="D22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>22.328700000000005</v>
       </c>
       <c r="E22" t="s">
@@ -3836,7 +3831,7 @@
         <v>19</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>35.409082126628576</v>
       </c>
       <c r="P22" t="s">
@@ -3854,7 +3849,7 @@
         <v>0.03</v>
       </c>
       <c r="D23" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13.397220000000001</v>
       </c>
       <c r="E23" t="s">
@@ -3887,7 +3882,7 @@
         <v>0.03</v>
       </c>
       <c r="D24" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13.397220000000001</v>
       </c>
       <c r="E24" t="s">
@@ -3905,22 +3900,22 @@
         <v>0.03</v>
       </c>
       <c r="D25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13.397220000000001</v>
       </c>
       <c r="E25" t="s">
         <v>12</v>
       </c>
-      <c r="V25" s="28" t="s">
+      <c r="V25" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="W25" s="25" t="s">
+      <c r="W25" s="20" t="s">
         <v>144</v>
       </c>
-      <c r="X25" s="25" t="s">
+      <c r="X25" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="Y25" s="25" t="s">
+      <c r="Y25" s="20" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3935,7 +3930,7 @@
         <v>0.03</v>
       </c>
       <c r="D26" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>13.397220000000001</v>
       </c>
       <c r="E26" t="s">
@@ -3944,20 +3939,20 @@
       <c r="G26" t="s">
         <v>149</v>
       </c>
-      <c r="V26" s="37">
+      <c r="V26" s="31">
         <f>+V17/$O17</f>
         <v>8.2935945749275666E-2</v>
       </c>
-      <c r="W26" s="37">
-        <f t="shared" ref="W26:Y26" si="14">+W17/$O17</f>
+      <c r="W26" s="31">
+        <f t="shared" ref="W26:Y26" si="16">+W17/$O17</f>
         <v>0.6223367089715629</v>
       </c>
-      <c r="X26" s="37">
-        <f t="shared" si="14"/>
+      <c r="X26" s="31">
+        <f t="shared" si="16"/>
         <v>0.20014218954130478</v>
       </c>
-      <c r="Y26" s="37">
-        <f t="shared" si="14"/>
+      <c r="Y26" s="31">
+        <f t="shared" si="16"/>
         <v>9.4585155737856683E-2</v>
       </c>
       <c r="Z26" s="4"/>
@@ -3973,7 +3968,7 @@
         <v>0.04</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>17.862960000000005</v>
       </c>
       <c r="E27" t="s">
@@ -3992,20 +3987,20 @@
         <f>+H27/SUM($H$27:$H$31)</f>
         <v>0.43782837127845886</v>
       </c>
-      <c r="V27" s="36">
-        <f t="shared" ref="V27:Y27" si="15">+V18/$O18</f>
+      <c r="V27" s="30">
+        <f t="shared" ref="V27:Y27" si="17">+V18/$O18</f>
         <v>0</v>
       </c>
-      <c r="W27" s="36">
-        <f t="shared" si="15"/>
+      <c r="W27" s="30">
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="X27" s="36">
-        <f t="shared" si="15"/>
+      <c r="X27" s="30">
+        <f t="shared" si="17"/>
         <v>0.67907573812580235</v>
       </c>
-      <c r="Y27" s="36">
-        <f t="shared" si="15"/>
+      <c r="Y27" s="30">
+        <f t="shared" si="17"/>
         <v>0.32092426187419765</v>
       </c>
       <c r="Z27" s="4"/>
@@ -4021,7 +4016,7 @@
         <v>0.04</v>
       </c>
       <c r="D28" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>17.862960000000005</v>
       </c>
       <c r="E28" t="s">
@@ -4037,23 +4032,23 @@
         <v>12</v>
       </c>
       <c r="J28" s="5">
-        <f t="shared" ref="J28:J31" si="16">+H28/SUM($H$27:$H$31)</f>
+        <f t="shared" ref="J28:J31" si="18">+H28/SUM($H$27:$H$31)</f>
         <v>0.36310566258026855</v>
       </c>
-      <c r="V28" s="36">
-        <f t="shared" ref="V28:Y28" si="17">+V19/$O19</f>
+      <c r="V28" s="30">
+        <f t="shared" ref="V28:Y28" si="19">+V19/$O19</f>
         <v>0</v>
       </c>
-      <c r="W28" s="36">
-        <f t="shared" si="17"/>
+      <c r="W28" s="30">
+        <f t="shared" si="19"/>
         <v>0.24191267043359946</v>
       </c>
-      <c r="X28" s="36">
-        <f t="shared" si="17"/>
+      <c r="X28" s="30">
+        <f t="shared" si="19"/>
         <v>0.51479871288912182</v>
       </c>
-      <c r="Y28" s="36">
-        <f t="shared" si="17"/>
+      <c r="Y28" s="30">
+        <f t="shared" si="19"/>
         <v>0.24328861667727872</v>
       </c>
       <c r="Z28" s="4"/>
@@ -4069,7 +4064,7 @@
         <v>0.02</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.9314800000000023</v>
       </c>
       <c r="E29" t="s">
@@ -4085,22 +4080,22 @@
         <v>12</v>
       </c>
       <c r="J29" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.17162872154115585</v>
       </c>
-      <c r="V29" s="36">
-        <f t="shared" ref="V29:W29" si="18">+V20/$O20</f>
+      <c r="V29" s="30">
+        <f t="shared" ref="V29:W29" si="20">+V20/$O20</f>
         <v>0</v>
       </c>
-      <c r="W29" s="36">
-        <f t="shared" si="18"/>
+      <c r="W29" s="30">
+        <f t="shared" si="20"/>
         <v>7.3051046942374423E-2</v>
       </c>
-      <c r="X29" s="36">
+      <c r="X29" s="30">
         <f>+X20/$O20</f>
         <v>0.62946854450254663</v>
       </c>
-      <c r="Y29" s="36">
+      <c r="Y29" s="30">
         <f>+Y20/$O20</f>
         <v>0.29748040855507879</v>
       </c>
@@ -4117,7 +4112,7 @@
         <v>0.02</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.9314800000000023</v>
       </c>
       <c r="E30" t="s">
@@ -4136,20 +4131,20 @@
         <f>+H30/SUM($H$27:$H$31)</f>
         <v>1.8680677174547577E-2</v>
       </c>
-      <c r="V30" s="38">
-        <f t="shared" ref="V30:Y30" si="19">+V21/$O21</f>
+      <c r="V30" s="32">
+        <f t="shared" ref="V30:Y30" si="21">+V21/$O21</f>
         <v>0</v>
       </c>
-      <c r="W30" s="38">
-        <f t="shared" si="19"/>
+      <c r="W30" s="32">
+        <f t="shared" si="21"/>
         <v>2.8464495819285934E-2</v>
       </c>
-      <c r="X30" s="38">
-        <f t="shared" si="19"/>
+      <c r="X30" s="32">
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="Y30" s="38">
-        <f t="shared" si="19"/>
+      <c r="Y30" s="32">
+        <f t="shared" si="21"/>
         <v>0.99409524014542738</v>
       </c>
       <c r="Z30" s="4"/>
@@ -4169,7 +4164,7 @@
         <v>12</v>
       </c>
       <c r="J31" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7565674255691769E-3</v>
       </c>
     </row>
@@ -4199,14 +4194,14 @@
         <v>112</v>
       </c>
       <c r="H35" s="4">
-        <f t="shared" ref="H35:H38" si="20">+$H$22*J28</f>
+        <f t="shared" ref="H35:H38" si="22">+$H$22*J28</f>
         <v>142.69512238178638</v>
       </c>
       <c r="I35" t="s">
         <v>12</v>
       </c>
       <c r="K35" s="7">
-        <f t="shared" ref="K35:K38" si="21">+(H35*365*24*0.0036/1000)/$D$3</f>
+        <f t="shared" ref="K35:K38" si="23">+(H35*365*24*0.0036/1000)/$D$3</f>
         <v>12.857238226948617</v>
       </c>
     </row>
@@ -4215,14 +4210,14 @@
         <v>113</v>
       </c>
       <c r="H36" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>67.447533730297721</v>
       </c>
       <c r="I36" t="s">
         <v>12</v>
       </c>
       <c r="K36" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>6.077215496339055</v>
       </c>
     </row>
@@ -4238,7 +4233,7 @@
         <v>12</v>
       </c>
       <c r="K37" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.6614656322545911</v>
       </c>
     </row>
@@ -4247,14 +4242,14 @@
         <v>115</v>
       </c>
       <c r="H38" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>3.4412007005253944</v>
       </c>
       <c r="I38" t="s">
         <v>12</v>
       </c>
       <c r="K38" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.31006201511933951</v>
       </c>
     </row>
@@ -4308,10 +4303,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A3:AL31"/>
+  <dimension ref="A3:AL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AI15" sqref="AI15:AK21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4337,7 +4332,7 @@
         <v>119</v>
       </c>
       <c r="D4" s="2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -4354,10 +4349,10 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B9" s="10"/>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="85"/>
       <c r="E9" s="10" t="s">
         <v>121</v>
       </c>
@@ -4380,31 +4375,31 @@
       </c>
       <c r="E10" s="10">
         <f>+C10*D4</f>
-        <v>83.25</v>
+        <v>111</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="10">
         <f>+E10*24*365/1000</f>
-        <v>729.27</v>
+        <v>972.36</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="4">
         <f>+G10*0.0036</f>
-        <v>2.625372</v>
+        <v>3.5004960000000001</v>
       </c>
       <c r="J10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="79" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="19"/>
+      <c r="D12" s="79"/>
       <c r="E12" t="s">
         <v>121</v>
       </c>
@@ -4425,60 +4420,60 @@
       </c>
       <c r="E13">
         <f t="shared" ref="E13:G13" si="0">+E10*$D$6</f>
-        <v>47.119500000000002</v>
+        <v>62.826000000000008</v>
       </c>
       <c r="F13" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>412.76682000000005</v>
+        <v>550.35576000000003</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
       </c>
       <c r="I13" s="6">
         <f>+G13*0.0036</f>
-        <v>1.4859605520000001</v>
+        <v>1.981280736</v>
       </c>
       <c r="J13" t="s">
         <v>19</v>
       </c>
-      <c r="Y13" s="52" t="s">
+      <c r="Y13" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="Z13" s="52"/>
-      <c r="AA13" s="52"/>
+      <c r="Z13" s="81"/>
+      <c r="AA13" s="81"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Y14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z14" s="19"/>
-      <c r="AA14" s="19"/>
+      <c r="Y14" s="79" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z14" s="79"/>
+      <c r="AA14" s="79"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="Y15" s="50">
+      <c r="Y15" s="44">
         <v>0.6</v>
       </c>
-      <c r="Z15" s="51">
+      <c r="Z15" s="45">
         <f>100%-Y15-AA15</f>
         <v>0.32</v>
       </c>
-      <c r="AA15" s="50">
+      <c r="AA15" s="44">
         <v>0.08</v>
       </c>
-      <c r="AE15" s="19" t="s">
+      <c r="AE15" s="79" t="s">
         <v>166</v>
       </c>
-      <c r="AF15" s="19"/>
-      <c r="AG15" s="19"/>
-      <c r="AI15" s="83" t="s">
+      <c r="AF15" s="79"/>
+      <c r="AG15" s="79"/>
+      <c r="AI15" s="87" t="s">
         <v>167</v>
       </c>
-      <c r="AJ15" s="84"/>
-      <c r="AK15" s="85"/>
-      <c r="AL15" s="53"/>
+      <c r="AJ15" s="88"/>
+      <c r="AK15" s="89"/>
+      <c r="AL15" s="46"/>
     </row>
     <row r="16" spans="1:38" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
@@ -4490,10 +4485,10 @@
       <c r="C16" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="86" t="s">
         <v>140</v>
       </c>
-      <c r="E16" s="22"/>
+      <c r="E16" s="86"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13" t="s">
         <v>120</v>
@@ -4502,14 +4497,14 @@
       <c r="L16" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22" t="s">
+      <c r="N16" s="86"/>
+      <c r="O16" s="86" t="s">
         <v>143</v>
       </c>
-      <c r="P16" s="22"/>
+      <c r="P16" s="86"/>
       <c r="R16" s="11" t="s">
         <v>155</v>
       </c>
@@ -4534,13 +4529,13 @@
       <c r="AG16" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="AI16" s="86" t="s">
+      <c r="AI16" s="71" t="s">
         <v>161</v>
       </c>
-      <c r="AJ16" s="87" t="s">
+      <c r="AJ16" s="72" t="s">
         <v>112</v>
       </c>
-      <c r="AK16" s="88" t="s">
+      <c r="AK16" s="73" t="s">
         <v>144</v>
       </c>
     </row>
@@ -4575,76 +4570,76 @@
         <v>3</v>
       </c>
       <c r="M17" s="7">
-        <f>+H17*$D$3*24*365*0.0036/1000</f>
-        <v>0.37446205910399999</v>
+        <f>+H17*$D$4*24*365*0.0036/1000</f>
+        <v>1.0698915974399998</v>
       </c>
       <c r="N17" t="s">
         <v>19</v>
       </c>
       <c r="O17" s="6">
         <f t="shared" ref="O17:O22" si="1">+M17/$D$3</f>
-        <v>1.0698915974400001</v>
+        <v>3.0568331355428571</v>
       </c>
       <c r="P17" t="s">
         <v>19</v>
       </c>
       <c r="R17">
-        <f>+Hoja2!F10+Hoja2!F25</f>
-        <v>0.374285714285715</v>
+        <f>+Hoja2!F25</f>
+        <v>0.24952380952381001</v>
       </c>
       <c r="S17" t="s">
         <v>19</v>
       </c>
-      <c r="T17" s="39">
+      <c r="T17" s="33">
         <f>+R17-M17</f>
-        <v>-1.7634481828499027E-4</v>
-      </c>
-      <c r="U17" s="39" t="s">
+        <v>-0.82036778791618981</v>
+      </c>
+      <c r="U17" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="V17" s="39"/>
+      <c r="V17" s="33"/>
       <c r="X17" t="s">
         <v>3</v>
       </c>
       <c r="Y17">
         <f>+$O17*Y$15</f>
-        <v>0.64193495846400006</v>
+        <v>1.8340998813257141</v>
       </c>
       <c r="Z17">
         <f t="shared" ref="Z17:AA21" si="2">+$O17*Z$15</f>
-        <v>0.34236531118080005</v>
+        <v>0.97818660337371433</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="2"/>
-        <v>8.5591327795200012E-2</v>
+        <f>+$O17*AA$15</f>
+        <v>0.24454665084342858</v>
       </c>
       <c r="AC17">
         <f>+SUM(Y17:AA17)</f>
-        <v>1.0698915974400001</v>
+        <v>3.0568331355428571</v>
       </c>
       <c r="AE17">
         <f>+Y17*0.35</f>
-        <v>0.22467723546240001</v>
+        <v>0.64193495846399995</v>
       </c>
       <c r="AF17">
         <f t="shared" ref="AF17:AG17" si="3">+Z17*0.35</f>
-        <v>0.11982785891328</v>
+        <v>0.34236531118079999</v>
       </c>
       <c r="AG17">
         <f t="shared" si="3"/>
-        <v>2.9956964728320001E-2</v>
-      </c>
-      <c r="AI17" s="89">
+        <v>8.5591327795199998E-2</v>
+      </c>
+      <c r="AI17" s="74">
         <f>+(AE17*1000/0.0036)/(365*24)</f>
-        <v>7.1244684000000005</v>
-      </c>
-      <c r="AJ17" s="90">
+        <v>20.355623999999995</v>
+      </c>
+      <c r="AJ17" s="69">
         <f t="shared" ref="AJ17:AK17" si="4">+(AF17*1000/0.0036)/(365*24)</f>
-        <v>3.7997164800000003</v>
-      </c>
-      <c r="AK17" s="91">
+        <v>10.856332800000001</v>
+      </c>
+      <c r="AK17" s="75">
         <f t="shared" si="4"/>
-        <v>0.94992912000000007</v>
+        <v>2.7140832000000001</v>
       </c>
     </row>
     <row r="18" spans="1:37" x14ac:dyDescent="0.25">
@@ -4668,7 +4663,7 @@
         <v>6</v>
       </c>
       <c r="H18" s="7">
-        <f t="shared" ref="H18:H21" si="6">+SUMIF($A$17:$A$30,G18,$D$17:$D$30)</f>
+        <f>+SUMIF($A$17:$A$30,G18,$D$17:$D$30)</f>
         <v>4.3978200000000012</v>
       </c>
       <c r="I18" t="s">
@@ -4678,7 +4673,7 @@
         <v>6</v>
       </c>
       <c r="M18" s="7">
-        <f t="shared" ref="M18:M21" si="7">+H18*$D$3*24*365*0.0036/1000</f>
+        <f>+H18*$D$3*24*365*0.0036/1000</f>
         <v>4.8541378032000017E-2</v>
       </c>
       <c r="N18" t="s">
@@ -4698,14 +4693,14 @@
       <c r="S18" t="s">
         <v>19</v>
       </c>
-      <c r="T18" s="39">
-        <f t="shared" ref="T18:T21" si="8">+R18-M18</f>
+      <c r="T18" s="33">
+        <f>+R18-M18</f>
         <v>0.32574433625371496</v>
       </c>
-      <c r="U18" s="39" t="s">
+      <c r="U18" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="V18" s="39"/>
+      <c r="V18" s="33"/>
       <c r="X18" t="s">
         <v>6</v>
       </c>
@@ -4721,31 +4716,31 @@
         <v>0</v>
       </c>
       <c r="AC18">
-        <f t="shared" ref="AC18:AC21" si="9">+SUM(Y18:AA18)</f>
+        <f t="shared" ref="AC18:AC21" si="6">+SUM(Y18:AA18)</f>
         <v>0.12759447939840007</v>
       </c>
       <c r="AE18">
-        <f t="shared" ref="AE18:AE21" si="10">+Y18*0.35</f>
+        <f>+Y18*0.35</f>
         <v>2.9124826819200013E-2</v>
       </c>
       <c r="AF18">
-        <f t="shared" ref="AF18:AF21" si="11">+Z18*0.35</f>
+        <f t="shared" ref="AF18:AF21" si="7">+Z18*0.35</f>
         <v>1.5533240970240008E-2</v>
       </c>
       <c r="AG18">
-        <f t="shared" ref="AG18:AG21" si="12">+AA18*0.35</f>
+        <f t="shared" ref="AG18:AG21" si="8">+AA18*0.35</f>
         <v>0</v>
       </c>
-      <c r="AI18" s="89">
-        <f t="shared" ref="AI18:AI21" si="13">+(AE18*1000/0.0036)/(365*24)</f>
+      <c r="AI18" s="74">
+        <f t="shared" ref="AI18:AI21" si="9">+(AE18*1000/0.0036)/(365*24)</f>
         <v>0.92354220000000042</v>
       </c>
-      <c r="AJ18" s="90">
-        <f t="shared" ref="AJ18:AJ21" si="14">+(AF18*1000/0.0036)/(365*24)</f>
+      <c r="AJ18" s="69">
+        <f t="shared" ref="AJ18:AJ21" si="10">+(AF18*1000/0.0036)/(365*24)</f>
         <v>0.4925558400000003</v>
       </c>
-      <c r="AK18" s="91">
-        <f t="shared" ref="AK18:AK21" si="15">+(AG18*1000/0.0036)/(365*24)</f>
+      <c r="AK18" s="75">
+        <f t="shared" ref="AK18:AK21" si="11">+(AG18*1000/0.0036)/(365*24)</f>
         <v>0</v>
       </c>
     </row>
@@ -4770,7 +4765,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="7">
-        <f t="shared" si="6"/>
+        <f>+SUMIF($A$17:$A$30,G19,$D$17:$D$30)</f>
         <v>11.308680000000001</v>
       </c>
       <c r="I19" t="s">
@@ -4780,7 +4775,7 @@
         <v>2</v>
       </c>
       <c r="M19" s="7">
-        <f t="shared" si="7"/>
+        <f>+H19*$D$3*24*365*0.0036/1000</f>
         <v>0.12482068636800001</v>
       </c>
       <c r="N19" t="s">
@@ -4800,19 +4795,19 @@
       <c r="S19" t="s">
         <v>19</v>
       </c>
-      <c r="T19" s="39">
-        <f t="shared" si="8"/>
+      <c r="T19" s="33">
+        <f>+R19-M19</f>
         <v>-0.10996313036624911</v>
       </c>
-      <c r="U19" s="39" t="s">
+      <c r="U19" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="V19" s="39"/>
+      <c r="V19" s="33"/>
       <c r="X19" t="s">
         <v>2</v>
       </c>
       <c r="Y19">
-        <f t="shared" ref="Y18:Y21" si="16">+$O19*Y$15</f>
+        <f>+$O19*Y$15</f>
         <v>0.21397831948800003</v>
       </c>
       <c r="Z19">
@@ -4820,35 +4815,35 @@
         <v>0.11412177039360001</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="2"/>
+        <f>+$O19*AA$15</f>
         <v>2.8530442598400003E-2</v>
       </c>
       <c r="AC19">
+        <f t="shared" si="6"/>
+        <v>0.35663053248000004</v>
+      </c>
+      <c r="AE19">
+        <f>+Y19*0.35</f>
+        <v>7.4892411820800003E-2</v>
+      </c>
+      <c r="AF19">
+        <f t="shared" si="7"/>
+        <v>3.9942619637760003E-2</v>
+      </c>
+      <c r="AG19">
+        <f t="shared" si="8"/>
+        <v>9.9856549094400008E-3</v>
+      </c>
+      <c r="AI19" s="74">
         <f t="shared" si="9"/>
-        <v>0.35663053248000004</v>
-      </c>
-      <c r="AE19">
+        <v>2.3748228000000005</v>
+      </c>
+      <c r="AJ19" s="69">
         <f t="shared" si="10"/>
-        <v>7.4892411820800003E-2</v>
-      </c>
-      <c r="AF19">
+        <v>1.2665721600000002</v>
+      </c>
+      <c r="AK19" s="75">
         <f t="shared" si="11"/>
-        <v>3.9942619637760003E-2</v>
-      </c>
-      <c r="AG19">
-        <f t="shared" si="12"/>
-        <v>9.9856549094400008E-3</v>
-      </c>
-      <c r="AI19" s="89">
-        <f t="shared" si="13"/>
-        <v>2.3748228000000005</v>
-      </c>
-      <c r="AJ19" s="90">
-        <f t="shared" si="14"/>
-        <v>1.2665721600000002</v>
-      </c>
-      <c r="AK19" s="91">
-        <f t="shared" si="15"/>
         <v>0.31664304000000004</v>
       </c>
     </row>
@@ -4873,7 +4868,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="7">
-        <f t="shared" si="6"/>
+        <f>+SUMIF($A$17:$A$30,G20,$D$17:$D$30)</f>
         <v>4.3978200000000012</v>
       </c>
       <c r="I20" t="s">
@@ -4883,7 +4878,7 @@
         <v>5</v>
       </c>
       <c r="M20" s="7">
-        <f t="shared" si="7"/>
+        <f>+H20*$D$3*24*365*0.0036/1000</f>
         <v>4.8541378032000017E-2</v>
       </c>
       <c r="N20" t="s">
@@ -4897,25 +4892,25 @@
         <v>19</v>
       </c>
       <c r="R20">
-        <f>+Hoja2!F29+Hoja2!F12</f>
-        <v>0.37428571428571483</v>
+        <f>+Hoja2!F29</f>
+        <v>0.32957550972273802</v>
       </c>
       <c r="S20" t="s">
         <v>19</v>
       </c>
-      <c r="T20" s="39">
-        <f t="shared" si="8"/>
-        <v>0.32574433625371479</v>
-      </c>
-      <c r="U20" s="39" t="s">
+      <c r="T20" s="33">
+        <f t="shared" ref="T18:T21" si="12">+R20-M20</f>
+        <v>0.28103413169073799</v>
+      </c>
+      <c r="U20" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="V20" s="39"/>
+      <c r="V20" s="33"/>
       <c r="X20" t="s">
         <v>5</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="16"/>
+        <f>+$O20*Y$15</f>
         <v>8.3213790912000041E-2</v>
       </c>
       <c r="Z20">
@@ -4923,35 +4918,35 @@
         <v>4.4380688486400026E-2</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="2"/>
+        <f>+$O20*AA$15</f>
         <v>1.1095172121600006E-2</v>
       </c>
       <c r="AC20">
+        <f t="shared" si="6"/>
+        <v>0.13868965152000007</v>
+      </c>
+      <c r="AE20">
+        <f>+Y20*0.35</f>
+        <v>2.9124826819200013E-2</v>
+      </c>
+      <c r="AF20">
+        <f t="shared" si="7"/>
+        <v>1.5533240970240008E-2</v>
+      </c>
+      <c r="AG20">
+        <f t="shared" si="8"/>
+        <v>3.8833102425600021E-3</v>
+      </c>
+      <c r="AI20" s="74">
         <f t="shared" si="9"/>
-        <v>0.13868965152000007</v>
-      </c>
-      <c r="AE20">
+        <v>0.92354220000000042</v>
+      </c>
+      <c r="AJ20" s="69">
         <f t="shared" si="10"/>
-        <v>2.9124826819200013E-2</v>
-      </c>
-      <c r="AF20">
+        <v>0.4925558400000003</v>
+      </c>
+      <c r="AK20" s="75">
         <f t="shared" si="11"/>
-        <v>1.5533240970240008E-2</v>
-      </c>
-      <c r="AG20">
-        <f t="shared" si="12"/>
-        <v>3.8833102425600021E-3</v>
-      </c>
-      <c r="AI20" s="89">
-        <f t="shared" si="13"/>
-        <v>0.92354220000000042</v>
-      </c>
-      <c r="AJ20" s="90">
-        <f t="shared" si="14"/>
-        <v>0.4925558400000003</v>
-      </c>
-      <c r="AK20" s="91">
-        <f t="shared" si="15"/>
         <v>0.12313896000000008</v>
       </c>
     </row>
@@ -4976,7 +4971,7 @@
         <v>4</v>
       </c>
       <c r="H21" s="15">
-        <f t="shared" si="6"/>
+        <f>+SUMIF($A$17:$A$30,G21,$D$17:$D$30)</f>
         <v>1.2565200000000001</v>
       </c>
       <c r="I21" s="14" t="s">
@@ -4986,7 +4981,7 @@
         <v>4</v>
       </c>
       <c r="M21" s="15">
-        <f t="shared" si="7"/>
+        <f>+H21*$D$3*24*365*0.0036/1000</f>
         <v>1.3868965152E-2</v>
       </c>
       <c r="N21" s="14" t="s">
@@ -5000,25 +4995,25 @@
         <v>19</v>
       </c>
       <c r="R21">
-        <f>+Hoja2!F16+Hoja2!F31</f>
-        <v>0.20023562499927339</v>
+        <f>+Hoja2!F31</f>
+        <v>7.5473720237368397E-2</v>
       </c>
       <c r="S21" t="s">
         <v>19</v>
       </c>
-      <c r="T21" s="39">
-        <f t="shared" si="8"/>
-        <v>0.18636665984727338</v>
-      </c>
-      <c r="U21" s="39" t="s">
+      <c r="T21" s="33">
+        <f t="shared" si="12"/>
+        <v>6.1604755085368397E-2</v>
+      </c>
+      <c r="U21" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="V21" s="39"/>
+      <c r="V21" s="33"/>
       <c r="X21" s="14" t="s">
         <v>4</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="16"/>
+        <f>+$O21*Y$15</f>
         <v>2.3775368831999998E-2</v>
       </c>
       <c r="Z21">
@@ -5026,35 +5021,35 @@
         <v>1.26801967104E-2</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="2"/>
+        <f>+$O21*AA$15</f>
         <v>3.1700491776000001E-3</v>
       </c>
       <c r="AC21">
+        <f t="shared" si="6"/>
+        <v>3.9625614719999994E-2</v>
+      </c>
+      <c r="AE21">
+        <f>+Y21*0.35</f>
+        <v>8.3213790911999992E-3</v>
+      </c>
+      <c r="AF21">
+        <f t="shared" si="7"/>
+        <v>4.4380688486400002E-3</v>
+      </c>
+      <c r="AG21">
+        <f t="shared" si="8"/>
+        <v>1.10951721216E-3</v>
+      </c>
+      <c r="AI21" s="76">
         <f t="shared" si="9"/>
-        <v>3.9625614719999994E-2</v>
-      </c>
-      <c r="AE21">
+        <v>0.26386919999999997</v>
+      </c>
+      <c r="AJ21" s="77">
         <f t="shared" si="10"/>
-        <v>8.3213790911999992E-3</v>
-      </c>
-      <c r="AF21">
+        <v>0.14073024000000001</v>
+      </c>
+      <c r="AK21" s="78">
         <f t="shared" si="11"/>
-        <v>4.4380688486400002E-3</v>
-      </c>
-      <c r="AG21">
-        <f t="shared" si="12"/>
-        <v>1.10951721216E-3</v>
-      </c>
-      <c r="AI21" s="92">
-        <f t="shared" si="13"/>
-        <v>0.26386919999999997</v>
-      </c>
-      <c r="AJ21" s="93">
-        <f t="shared" si="14"/>
-        <v>0.14073024000000001</v>
-      </c>
-      <c r="AK21" s="94">
-        <f t="shared" si="15"/>
         <v>3.5182560000000002E-2</v>
       </c>
     </row>
@@ -5087,14 +5082,14 @@
       </c>
       <c r="M22" s="7">
         <f>+SUM(M17:M21)</f>
-        <v>0.61023446668799997</v>
+        <v>1.305664005024</v>
       </c>
       <c r="N22" t="s">
         <v>19</v>
       </c>
       <c r="O22" s="6">
         <f t="shared" si="1"/>
-        <v>1.74352704768</v>
+        <v>3.7304685857828574</v>
       </c>
       <c r="P22" t="s">
         <v>19</v>
@@ -5119,15 +5114,15 @@
       </c>
       <c r="AI23" s="7">
         <f>+SUM(AI17:AI21)</f>
-        <v>11.610244800000002</v>
+        <v>24.841400399999994</v>
       </c>
       <c r="AJ23" s="7">
-        <f t="shared" ref="AJ23:AK23" si="17">+SUM(AJ17:AJ21)</f>
-        <v>6.1921305600000007</v>
+        <f t="shared" ref="AJ23:AK23" si="13">+SUM(AJ17:AJ21)</f>
+        <v>13.248746880000001</v>
       </c>
       <c r="AK23" s="7">
-        <f t="shared" si="17"/>
-        <v>1.4248936800000003</v>
+        <f t="shared" si="13"/>
+        <v>3.1890477600000002</v>
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.25">
@@ -5147,11 +5142,16 @@
       <c r="E24" t="s">
         <v>12</v>
       </c>
-      <c r="T24" s="39">
+      <c r="M24" s="7"/>
+      <c r="R24">
+        <f>+SUM(R17:R21)</f>
+        <v>1.0437163097713822</v>
+      </c>
+      <c r="T24" s="33">
         <f>+T21+T20+T18</f>
-        <v>0.83785533235470311</v>
-      </c>
-      <c r="U24" s="39" t="s">
+        <v>0.66838322302982134</v>
+      </c>
+      <c r="U24" s="33" t="s">
         <v>163</v>
       </c>
     </row>
@@ -5174,9 +5174,9 @@
       </c>
       <c r="T25">
         <f>+T24*44</f>
-        <v>36.865634623606937</v>
-      </c>
-      <c r="U25" s="39" t="s">
+        <v>29.408861813312139</v>
+      </c>
+      <c r="U25" s="33" t="s">
         <v>164</v>
       </c>
     </row>
@@ -5233,6 +5233,14 @@
       <c r="E28" t="s">
         <v>12</v>
       </c>
+      <c r="H28" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="I28" s="81"/>
+      <c r="J28" s="81"/>
+      <c r="Q28" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -5251,6 +5259,18 @@
       <c r="E29" t="s">
         <v>12</v>
       </c>
+      <c r="H29" s="79" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="P29" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q29">
+        <f>+Hoja1!G56</f>
+        <v>9.8346473268648609</v>
+      </c>
     </row>
     <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
@@ -5268,6 +5288,19 @@
       </c>
       <c r="E30" t="s">
         <v>12</v>
+      </c>
+      <c r="H30" s="44">
+        <v>0.6</v>
+      </c>
+      <c r="I30" s="45">
+        <f>100%-H30-J30</f>
+        <v>0.32</v>
+      </c>
+      <c r="J30" s="44">
+        <v>0.08</v>
+      </c>
+      <c r="P30" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:37" x14ac:dyDescent="0.25">
@@ -5276,18 +5309,124 @@
         <f>+SUM(C17:C30)</f>
         <v>1.0000000000000002</v>
       </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="P31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32">
+        <f>+$H17*H$30</f>
+        <v>20.355623999999999</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32:J32" si="14">+$H17*I$30</f>
+        <v>10.856332800000001</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="14"/>
+        <v>2.7140832000000001</v>
+      </c>
+      <c r="P32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ref="H33:J33" si="15">+$H18*H$30</f>
+        <v>2.6386920000000007</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="15"/>
+        <v>1.4073024000000005</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="15"/>
+        <v>0.35182560000000013</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ref="H34:J34" si="16">+$H19*H$30</f>
+        <v>6.7852079999999999</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="16"/>
+        <v>3.6187776000000005</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="16"/>
+        <v>0.90469440000000012</v>
+      </c>
+    </row>
+    <row r="35" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>5</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ref="H35:J35" si="17">+$H20*H$30</f>
+        <v>2.6386920000000007</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="17"/>
+        <v>1.4073024000000005</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="17"/>
+        <v>0.35182560000000013</v>
+      </c>
+    </row>
+    <row r="36" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G36" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ref="H36:J36" si="18">+$H21*H$30</f>
+        <v>0.75391200000000003</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="18"/>
+        <v>0.40208640000000001</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="18"/>
+        <v>0.1005216</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="Y13:AA13"/>
+  <mergeCells count="11">
+    <mergeCell ref="H29:J29"/>
     <mergeCell ref="AE15:AG15"/>
     <mergeCell ref="AI15:AK15"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C12:D12"/>
+    <mergeCell ref="H28:J28"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="M16:N16"/>
     <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="Y13:AA13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5303,7 +5442,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5690,10 +5829,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174DA97B-0B9C-471D-9BAA-37CFD4E0FD71}">
-  <dimension ref="D9:J78"/>
+  <dimension ref="D9:L78"/>
   <sheetViews>
-    <sheetView topLeftCell="B52" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="L73" sqref="L73:L74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6309,7 +6448,7 @@
         <v>0.45154082596841399</v>
       </c>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
         <v>27</v>
       </c>
@@ -6323,7 +6462,7 @@
         <v>30.106735962689498</v>
       </c>
     </row>
-    <row r="66" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
         <v>27</v>
       </c>
@@ -6337,7 +6476,7 @@
         <v>0.13373317447933</v>
       </c>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D67" t="s">
         <v>27</v>
       </c>
@@ -6351,7 +6490,7 @@
         <v>11.3323595016805</v>
       </c>
     </row>
-    <row r="70" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D70" t="s">
         <v>22</v>
       </c>
@@ -6359,7 +6498,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
         <v>24</v>
       </c>
@@ -6373,7 +6512,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="72" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D72" t="s">
         <v>27</v>
       </c>
@@ -6394,7 +6533,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D73" t="s">
         <v>27</v>
       </c>
@@ -6407,8 +6546,12 @@
       <c r="G73">
         <v>4.33070909751605</v>
       </c>
-    </row>
-    <row r="74" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="L73">
+        <f>+G73</f>
+        <v>4.33070909751605</v>
+      </c>
+    </row>
+    <row r="74" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D74" t="s">
         <v>27</v>
       </c>
@@ -6421,8 +6564,12 @@
       <c r="G74">
         <v>10.9185152593786</v>
       </c>
-    </row>
-    <row r="75" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="L74">
+        <f>+G74</f>
+        <v>10.9185152593786</v>
+      </c>
+    </row>
+    <row r="75" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D75" t="s">
         <v>27</v>
       </c>
@@ -6443,7 +6590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="76" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D76" t="s">
         <v>27</v>
       </c>
@@ -6457,7 +6604,7 @@
         <v>2.4929417117336898</v>
       </c>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D77" t="s">
         <v>27</v>
       </c>
@@ -6471,7 +6618,7 @@
         <v>0.45154082596841399</v>
       </c>
     </row>
-    <row r="78" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D78" t="s">
         <v>27</v>
       </c>
@@ -6509,97 +6656,97 @@
       </c>
     </row>
     <row r="4" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="F4" s="60" t="s">
+      <c r="F4" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="F5" s="61" t="s">
+      <c r="F5" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="H5" s="23" t="s">
+      <c r="H5" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="19" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E6" s="62" t="s">
+      <c r="E6" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="63">
+      <c r="F6" s="55">
         <v>19.999999999999996</v>
       </c>
-      <c r="G6" s="63">
+      <c r="G6" s="55">
         <v>150.07647247502405</v>
       </c>
-      <c r="H6" s="63">
+      <c r="H6" s="55">
         <v>48.264281002198075</v>
       </c>
-      <c r="I6" s="64">
+      <c r="I6" s="56">
         <v>22.809206522777917</v>
       </c>
     </row>
     <row r="7" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="57">
+      <c r="F7" s="7">
         <v>0</v>
       </c>
-      <c r="G7" s="57">
+      <c r="G7" s="7">
         <v>0</v>
       </c>
-      <c r="H7" s="57">
+      <c r="H7" s="7">
         <v>21.228029807445445</v>
       </c>
-      <c r="I7" s="58">
+      <c r="I7" s="50">
         <v>10.032150192554559</v>
       </c>
     </row>
     <row r="8" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E8" s="65" t="s">
+      <c r="E8" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="57">
+      <c r="F8" s="7">
         <v>0</v>
       </c>
-      <c r="G8" s="57">
+      <c r="G8" s="7">
         <v>19.445743599518565</v>
       </c>
-      <c r="H8" s="57">
+      <c r="H8" s="7">
         <v>41.381229673754405</v>
       </c>
-      <c r="I8" s="58">
+      <c r="I8" s="50">
         <v>19.556346726727035</v>
       </c>
     </row>
     <row r="9" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E9" s="65" t="s">
+      <c r="E9" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="7">
         <v>0</v>
       </c>
-      <c r="G9" s="57">
+      <c r="G9" s="7">
         <v>2.2835888766070749</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="7">
         <v>19.677300005487623</v>
       </c>
-      <c r="I9" s="58">
+      <c r="I9" s="50">
         <v>9.2992911179053053</v>
       </c>
     </row>
     <row r="10" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="58" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="15">
@@ -6611,7 +6758,7 @@
       <c r="H10" s="15">
         <v>0</v>
       </c>
-      <c r="I10" s="59">
+      <c r="I10" s="51">
         <v>8.8787417554540831</v>
       </c>
     </row>
@@ -6619,17 +6766,17 @@
       <c r="E14" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="70"/>
-      <c r="K14" s="70" t="s">
+      <c r="J14" s="62"/>
+      <c r="K14" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="L14" s="70" t="s">
+      <c r="L14" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="70" t="s">
+      <c r="M14" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="N14" s="70"/>
+      <c r="N14" s="62"/>
       <c r="O14" t="s">
         <v>169</v>
       </c>
@@ -6641,26 +6788,26 @@
       </c>
     </row>
     <row r="15" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E15" s="67" t="s">
+      <c r="E15" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="F15" s="68"/>
-      <c r="G15" s="69"/>
-      <c r="J15" s="71" t="s">
+      <c r="F15" s="60"/>
+      <c r="G15" s="61"/>
+      <c r="J15" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="K15" s="72">
+      <c r="K15" s="64">
         <f>+SUM(F6:F10)</f>
         <v>19.999999999999996</v>
       </c>
-      <c r="L15" s="70">
+      <c r="L15" s="62">
         <v>0</v>
       </c>
-      <c r="M15" s="72">
+      <c r="M15" s="64">
         <f>+L15+K15</f>
         <v>19.999999999999996</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="N15" s="62" t="s">
         <v>12</v>
       </c>
       <c r="O15">
@@ -6677,31 +6824,31 @@
       </c>
     </row>
     <row r="16" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="F16" s="55" t="s">
+      <c r="F16" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="J16" s="73" t="s">
+      <c r="J16" s="65" t="s">
         <v>161</v>
       </c>
-      <c r="K16" s="72">
+      <c r="K16" s="64">
         <f>+SUM(I6:I10)</f>
         <v>70.575736315418894</v>
       </c>
-      <c r="L16" s="72">
+      <c r="L16" s="64">
         <f>+SUM(E17:E21)</f>
         <v>11.610244800000002</v>
       </c>
-      <c r="M16" s="72">
+      <c r="M16" s="64">
         <f t="shared" ref="M16:M18" si="0">+L16+K16</f>
         <v>82.185981115418898</v>
       </c>
-      <c r="N16" s="70" t="s">
+      <c r="N16" s="62" t="s">
         <v>12</v>
       </c>
       <c r="O16">
@@ -6722,31 +6869,31 @@
       </c>
     </row>
     <row r="17" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E17" s="26">
+      <c r="E17" s="21">
         <v>7.1244684000000005</v>
       </c>
-      <c r="F17" s="57">
+      <c r="F17" s="7">
         <v>3.7997164800000003</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="50">
         <v>0.94992912000000007</v>
       </c>
-      <c r="J17" s="71" t="s">
+      <c r="J17" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="K17" s="72">
+      <c r="K17" s="64">
         <f>+SUM(H6:H10)</f>
         <v>130.55084048888557</v>
       </c>
-      <c r="L17" s="72">
+      <c r="L17" s="64">
         <f>+SUM(F17:F21)</f>
         <v>6.1921305600000007</v>
       </c>
-      <c r="M17" s="72">
+      <c r="M17" s="64">
         <f t="shared" si="0"/>
         <v>136.74297104888558</v>
       </c>
-      <c r="N17" s="70" t="s">
+      <c r="N17" s="62" t="s">
         <v>12</v>
       </c>
       <c r="O17">
@@ -6767,31 +6914,31 @@
       </c>
     </row>
     <row r="18" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E18" s="26">
+      <c r="E18" s="21">
         <v>0.92354220000000042</v>
       </c>
-      <c r="F18" s="57">
+      <c r="F18" s="7">
         <v>0.4925558400000003</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="50">
         <v>0</v>
       </c>
-      <c r="J18" s="71" t="s">
+      <c r="J18" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="K18" s="72">
+      <c r="K18" s="64">
         <f>+SUM(G6:G10)</f>
         <v>172.0600350262697</v>
       </c>
-      <c r="L18" s="72">
+      <c r="L18" s="64">
         <f>+SUM(G17:G21)</f>
         <v>1.4248936800000003</v>
       </c>
-      <c r="M18" s="72">
+      <c r="M18" s="64">
         <f t="shared" si="0"/>
         <v>173.4849287062697</v>
       </c>
-      <c r="N18" s="70" t="s">
+      <c r="N18" s="62" t="s">
         <v>12</v>
       </c>
       <c r="O18">
@@ -6812,13 +6959,13 @@
       </c>
     </row>
     <row r="19" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E19" s="26">
+      <c r="E19" s="21">
         <v>2.3748228000000005</v>
       </c>
-      <c r="F19" s="57">
+      <c r="F19" s="7">
         <v>1.2665721600000002</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="50">
         <v>0.31664304000000004</v>
       </c>
       <c r="S19" t="s">
@@ -6832,24 +6979,24 @@
       </c>
     </row>
     <row r="20" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E20" s="26">
+      <c r="E20" s="21">
         <v>0.92354220000000042</v>
       </c>
-      <c r="F20" s="57">
+      <c r="F20" s="7">
         <v>0.4925558400000003</v>
       </c>
-      <c r="G20" s="58">
+      <c r="G20" s="50">
         <v>0.12313896000000008</v>
       </c>
     </row>
     <row r="21" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E21" s="27">
+      <c r="E21" s="22">
         <v>0.26386919999999997</v>
       </c>
       <c r="F21" s="15">
         <v>0.14073024000000001</v>
       </c>
-      <c r="G21" s="59">
+      <c r="G21" s="51">
         <v>3.5182560000000002E-2</v>
       </c>
     </row>

</xml_diff>